<commit_message>
Correct control column CDOM data
</commit_message>
<xml_diff>
--- a/Data/Column Experiment Data/2025_control_col_data/CDOM/7_Spectral indices/SpectralIndices_combined_sample_only_DOC_norm.xlsx
+++ b/Data/Column Experiment Data/2025_control_col_data/CDOM/7_Spectral indices/SpectralIndices_combined_sample_only_DOC_norm.xlsx
@@ -626,7 +626,7 @@
         <v>0.173688611989615</v>
       </c>
       <c r="U2">
-        <v>0.0233372030866255</v>
+        <v>0.0411267193744868</v>
       </c>
       <c r="V2">
         <v>0.0162496592554788</v>
@@ -752,7 +752,7 @@
         <v>0.7576276181729</v>
       </c>
       <c r="U3">
-        <v>0.0554459265530136</v>
+        <v>0.137754879693119</v>
       </c>
       <c r="V3">
         <v>0.0530787792681102</v>
@@ -878,7 +878,7 @@
         <v>0.734930691226288</v>
       </c>
       <c r="U4">
-        <v>0.0549321852372344</v>
+        <v>0.142288767825704</v>
       </c>
       <c r="V4">
         <v>0.0522661368355983</v>
@@ -1004,7 +1004,7 @@
         <v>0.141268851846325</v>
       </c>
       <c r="U5">
-        <v>0.0231132076802698</v>
+        <v>0.0276048100308799</v>
       </c>
       <c r="V5">
         <v>0.0247869092734518</v>
@@ -1130,7 +1130,7 @@
         <v>0.260775990348604</v>
       </c>
       <c r="U6">
-        <v>0.0136562051028557</v>
+        <v>0.0159410217066824</v>
       </c>
       <c r="V6">
         <v>0.0235283902094423</v>
@@ -1256,7 +1256,7 @@
         <v>0.282385785731768</v>
       </c>
       <c r="U7">
-        <v>0.0140161219282469</v>
+        <v>0.0160903776484691</v>
       </c>
       <c r="V7">
         <v>0.0240249394680916</v>
@@ -1382,7 +1382,7 @@
         <v>0.263009606607922</v>
       </c>
       <c r="U8">
-        <v>0.0139968017147352</v>
+        <v>0.0169110427241819</v>
       </c>
       <c r="V8">
         <v>0.0226076167414737</v>
@@ -1508,7 +1508,7 @@
         <v>0.242239305926093</v>
       </c>
       <c r="U9">
-        <v>0.0192786386919215</v>
+        <v>0.0221480982502538</v>
       </c>
       <c r="V9">
         <v>0.0266429435513533</v>
@@ -1634,7 +1634,7 @@
         <v>0.247357510592629</v>
       </c>
       <c r="U10">
-        <v>0.0178815872052009</v>
+        <v>0.0203145574392796</v>
       </c>
       <c r="V10">
         <v>0.0261240300553191</v>
@@ -1760,7 +1760,7 @@
         <v>0.255443509319384</v>
       </c>
       <c r="U11">
-        <v>0.016004314737657</v>
+        <v>0.0169569612602203</v>
       </c>
       <c r="V11">
         <v>0.0251444999001471</v>
@@ -1886,7 +1886,7 @@
         <v>0.24681871320376</v>
       </c>
       <c r="U12">
-        <v>0.0159466058332136</v>
+        <v>0.0183971149351745</v>
       </c>
       <c r="V12">
         <v>0.0240376633328054</v>
@@ -2012,7 +2012,7 @@
         <v>0.286548450427634</v>
       </c>
       <c r="U13">
-        <v>0.0137297508578609</v>
+        <v>0.0164253374616337</v>
       </c>
       <c r="V13">
         <v>0.0232311010979487</v>
@@ -2264,7 +2264,7 @@
         <v>0.2724214615737</v>
       </c>
       <c r="U15">
-        <v>0.0149996907148733</v>
+        <v>0.0167169698854419</v>
       </c>
       <c r="V15">
         <v>0.0245315396323562</v>
@@ -2390,7 +2390,7 @@
         <v>0.259757684490201</v>
       </c>
       <c r="U16">
-        <v>0.0143853221530144</v>
+        <v>0.0178324621273998</v>
       </c>
       <c r="V16">
         <v>0.0238597012159221</v>
@@ -2516,7 +2516,7 @@
         <v>0.760572077169208</v>
       </c>
       <c r="U17">
-        <v>0.0530564548154544</v>
+        <v>0.12486974314811</v>
       </c>
       <c r="V17">
         <v>0.0520517899907631</v>
@@ -2642,7 +2642,7 @@
         <v>0.177690399092595</v>
       </c>
       <c r="U18">
-        <v>0.0218488518937789</v>
+        <v>0.0288555822700065</v>
       </c>
       <c r="V18">
         <v>0.0271293071324727</v>
@@ -2894,7 +2894,7 @@
         <v>0.34883577970382</v>
       </c>
       <c r="U20">
-        <v>0.01288340483665</v>
+        <v>0.0165825139414517</v>
       </c>
       <c r="V20">
         <v>0.0254717031756231</v>
@@ -3020,7 +3020,7 @@
         <v>0.329586294258818</v>
       </c>
       <c r="U21">
-        <v>0.0112873080818368</v>
+        <v>0.0130265704213584</v>
       </c>
       <c r="V21">
         <v>0.0236064553354574</v>
@@ -3398,7 +3398,7 @@
         <v>0.297839754273116</v>
       </c>
       <c r="U24">
-        <v>0.0133387384107744</v>
+        <v>0.0145134055811091</v>
       </c>
       <c r="V24">
         <v>0.0249764053204342</v>
@@ -3524,7 +3524,7 @@
         <v>0.32454181432647</v>
       </c>
       <c r="U25">
-        <v>0.0123922976967172</v>
+        <v>0.0176315629795187</v>
       </c>
       <c r="V25">
         <v>0.0242259960972264</v>
@@ -3650,7 +3650,7 @@
         <v>0.337813709615552</v>
       </c>
       <c r="U26">
-        <v>0.0114818019127583</v>
+        <v>0.014983506100398</v>
       </c>
       <c r="V26">
         <v>0.0244238209733325</v>
@@ -3776,7 +3776,7 @@
         <v>0.344000742190446</v>
       </c>
       <c r="U27">
-        <v>0.0118414915481715</v>
+        <v>0.0150749117426301</v>
       </c>
       <c r="V27">
         <v>0.0240030731503111</v>
@@ -3902,7 +3902,7 @@
         <v>0.364982018554088</v>
       </c>
       <c r="U28">
-        <v>0.0118286813712345</v>
+        <v>0.0148432692447322</v>
       </c>
       <c r="V28">
         <v>0.0223703582308374</v>
@@ -4154,7 +4154,7 @@
         <v>0.689534729408384</v>
       </c>
       <c r="U30">
-        <v>0.0555679511558875</v>
+        <v>0.138285682389224</v>
       </c>
       <c r="V30">
         <v>0.0552357682965265</v>
@@ -4280,7 +4280,7 @@
         <v>0.08916857620110009</v>
       </c>
       <c r="U31">
-        <v>0.028277091292912</v>
+        <v>0.0384269901255294</v>
       </c>
       <c r="V31">
         <v>0.0252769125919876</v>
@@ -4406,7 +4406,7 @@
         <v>0.101336478906914</v>
       </c>
       <c r="U32">
-        <v>0.0154887541571256</v>
+        <v>0.015682766662076</v>
       </c>
       <c r="V32">
         <v>0.0243248192578065</v>
@@ -4784,7 +4784,7 @@
         <v>0.136024795230284</v>
       </c>
       <c r="U35">
-        <v>0.022446062804363</v>
+        <v>0.0257194071524935</v>
       </c>
       <c r="V35">
         <v>0.029975695923329</v>
@@ -4910,7 +4910,7 @@
         <v>0.128532623131774</v>
       </c>
       <c r="U36">
-        <v>0.020205112232345</v>
+        <v>0.022271862737421</v>
       </c>
       <c r="V36">
         <v>0.0270628684477376</v>
@@ -5792,7 +5792,7 @@
         <v>0.848174939747864</v>
       </c>
       <c r="U43">
-        <v>0.0597448338182254</v>
+        <v>0.114751473436286</v>
       </c>
       <c r="V43">
         <v>0.0598887224822597</v>
@@ -5918,7 +5918,7 @@
         <v>0.309170685247686</v>
       </c>
       <c r="U44">
-        <v>0.0275164997358956</v>
+        <v>0.049990096433465</v>
       </c>
       <c r="V44">
         <v>0.0310185304468522</v>
@@ -6044,7 +6044,7 @@
         <v>0.465142187466444</v>
       </c>
       <c r="U45">
-        <v>0.0148803601876084</v>
+        <v>0.0185137536535827</v>
       </c>
       <c r="V45">
         <v>0.0193835628620498</v>
@@ -6170,7 +6170,7 @@
         <v>0.486925646379938</v>
       </c>
       <c r="U46">
-        <v>0.0134419021198919</v>
+        <v>0.0165529657541441</v>
       </c>
       <c r="V46">
         <v>0.0181252476865588</v>
@@ -6296,7 +6296,7 @@
         <v>0.483123050710628</v>
       </c>
       <c r="U47">
-        <v>0.0151535030058376</v>
+        <v>0.0201357834504918</v>
       </c>
       <c r="V47">
         <v>0.0188704439531975</v>
@@ -6422,7 +6422,7 @@
         <v>0.451574820834752</v>
       </c>
       <c r="U48">
-        <v>0.0163719410697922</v>
+        <v>0.0274770942794866</v>
       </c>
       <c r="V48">
         <v>0.0214967255614624</v>
@@ -6548,7 +6548,7 @@
         <v>0.5105121331093</v>
       </c>
       <c r="U49">
-        <v>0.0157970295874126</v>
+        <v>0.0262211304957483</v>
       </c>
       <c r="V49">
         <v>0.0219855750828755</v>
@@ -6674,7 +6674,7 @@
         <v>0.524638502578618</v>
       </c>
       <c r="U50">
-        <v>0.0162977152972101</v>
+        <v>0.0198702336873087</v>
       </c>
       <c r="V50">
         <v>0.0199269620983209</v>
@@ -6800,7 +6800,7 @@
         <v>0.526074246395614</v>
       </c>
       <c r="U51">
-        <v>0.0141242356509554</v>
+        <v>0.0188136883612113</v>
       </c>
       <c r="V51">
         <v>0.0172772615278944</v>
@@ -6926,7 +6926,7 @@
         <v>0.490932778265</v>
       </c>
       <c r="U52">
-        <v>0.0157242114838434</v>
+        <v>0.0210278660915613</v>
       </c>
       <c r="V52">
         <v>0.0177972813873417</v>
@@ -7052,7 +7052,7 @@
         <v>0.5170535162015441</v>
       </c>
       <c r="U53">
-        <v>0.016902958575475</v>
+        <v>0.0221193188753883</v>
       </c>
       <c r="V53">
         <v>0.0200947836733576</v>
@@ -7178,7 +7178,7 @@
         <v>0.448029992095022</v>
       </c>
       <c r="U54">
-        <v>0.0151244875741607</v>
+        <v>0.0205918091192174</v>
       </c>
       <c r="V54">
         <v>0.0176543923633545</v>
@@ -7304,7 +7304,7 @@
         <v>0.471335676788338</v>
       </c>
       <c r="U55">
-        <v>0.0153071870993973</v>
+        <v>0.0207059825985176</v>
       </c>
       <c r="V55">
         <v>0.0178399841749268</v>
@@ -7430,7 +7430,7 @@
         <v>0.801530035471152</v>
       </c>
       <c r="U56">
-        <v>0.0555744670972267</v>
+        <v>0.141527248449506</v>
       </c>
       <c r="V56">
         <v>0.052998559897695</v>
@@ -7556,7 +7556,7 @@
         <v>0.193263771057744</v>
       </c>
       <c r="U57">
-        <v>0.0358051896608496</v>
+        <v>0.0508129870452514</v>
       </c>
       <c r="V57">
         <v>0.0294039336858702</v>
@@ -7682,7 +7682,7 @@
         <v>0.222134600086702</v>
       </c>
       <c r="U58">
-        <v>0.0153525999842072</v>
+        <v>0.018266266152601</v>
       </c>
       <c r="V58">
         <v>0.0233508319717046</v>
@@ -7808,7 +7808,7 @@
         <v>0.250038837854454</v>
       </c>
       <c r="U59">
-        <v>0.0156622738226844</v>
+        <v>0.0190956504508666</v>
       </c>
       <c r="V59">
         <v>0.0235509880806291</v>
@@ -7934,7 +7934,7 @@
         <v>0.208966913989343</v>
       </c>
       <c r="U60">
-        <v>0.0130870928350504</v>
+        <v>0.0143705557927447</v>
       </c>
       <c r="V60">
         <v>0.0199663474469336</v>
@@ -8060,7 +8060,7 @@
         <v>0.242611425588882</v>
       </c>
       <c r="U61">
-        <v>0.0196287053345869</v>
+        <v>0.025486775160914</v>
       </c>
       <c r="V61">
         <v>0.0225103601245671</v>
@@ -8186,7 +8186,7 @@
         <v>0.24824727908894</v>
       </c>
       <c r="U62">
-        <v>0.0178909889591417</v>
+        <v>0.0230486848737979</v>
       </c>
       <c r="V62">
         <v>0.0236841027829584</v>
@@ -8312,7 +8312,7 @@
         <v>0.241110483793947</v>
       </c>
       <c r="U63">
-        <v>0.018061658338739</v>
+        <v>0.0229091568475681</v>
       </c>
       <c r="V63">
         <v>0.023273814889798</v>
@@ -8438,7 +8438,7 @@
         <v>0.229300106984263</v>
       </c>
       <c r="U64">
-        <v>0.0165291601373818</v>
+        <v>0.0205571905932622</v>
       </c>
       <c r="V64">
         <v>0.0216512076216562</v>
@@ -8564,7 +8564,7 @@
         <v>0.2443285140442</v>
       </c>
       <c r="U65">
-        <v>0.0178852173371773</v>
+        <v>0.0228505301089434</v>
       </c>
       <c r="V65">
         <v>0.0228349251245561</v>
@@ -8690,7 +8690,7 @@
         <v>0.250557958823767</v>
       </c>
       <c r="U66">
-        <v>0.0163062970063055</v>
+        <v>0.0195030516029249</v>
       </c>
       <c r="V66">
         <v>0.0210611146867178</v>
@@ -8816,7 +8816,7 @@
         <v>0.246156077663847</v>
       </c>
       <c r="U67">
-        <v>0.0128908211805383</v>
+        <v>0.0138982294802812</v>
       </c>
       <c r="V67">
         <v>0.0222747975992199</v>
@@ -8942,7 +8942,7 @@
         <v>0.221465473866441</v>
       </c>
       <c r="U68">
-        <v>0.0149002417489321</v>
+        <v>0.0178372356582628</v>
       </c>
       <c r="V68">
         <v>0.0226523246748194</v>

</xml_diff>